<commit_message>
Criado modelo que baixa o relatório de desdobramentos do email, renomeando-o para servir de base ao código unificado. Correção do modelo de smartimport para tirar warningalerts
</commit_message>
<xml_diff>
--- a/Correcao EPROC/Lista de notas.xlsx
+++ b/Correcao EPROC/Lista de notas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,177 +571,42 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5056780-46.2019.8.21.0001</t>
+          <t>5002019-61.2019.8.21.0067</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0140462-81.2019.8.21.0001</t>
+          <t>0064471-68.2019.8.21.9000</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Digitalizado</t>
+          <t>Relacionado na TR</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Sem dados de processo originário 2</t>
+          <t>0042940-86.2020.8.21.9000</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Nulo</t>
+          <t>Relacionado na TR</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Sem dados de processo originário 3</t>
+          <t>9000401-13.2019.8.21.0067</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Nulo</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>14/08/2019</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>5000559-78.2019.8.21.0054</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0003337-09.2019.8.21.0054</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Digitalizado</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>03/09/2019</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>5001387-66.2023.8.21.9000</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>5008039-43.2018.8.21.0022</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Originário</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>15/02/2023</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>5009986-45.2011.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>0323125-76.2011.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Digitalizado</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>14/09/2011</t>
+          <t>27/05/2019</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Construção do código para enviar resultado por email
</commit_message>
<xml_diff>
--- a/Correcao EPROC/Lista de notas.xlsx
+++ b/Correcao EPROC/Lista de notas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,42 +571,312 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5002019-61.2019.8.21.0067</t>
+          <t>5010754-58.2017.8.21.0001</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0064471-68.2019.8.21.9000</t>
+          <t>0196807-38.2017.8.21.0001</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>10/11/2017</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>5008281-41.2013.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0087776-25.2013.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>26/12/2011</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>5001221-76.2018.8.21.0054</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0066578-85.2019.8.21.9000</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>Relacionado na TR</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0042940-86.2020.8.21.9000</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Relacionado na TR</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>9000401-13.2019.8.21.0067</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>9000149-83.2018.8.21.0054</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>Migrado</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>27/05/2019</t>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>13/03/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>5006432-89.2018.8.21.0023</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>9003986-45.2018.8.21.0023</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>31/10/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>5006429-37.2018.8.21.0023</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>9003787-23.2018.8.21.0023</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>17/10/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>5009614-96.2011.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0420415-91.2011.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>07/12/2011</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>5033806-25.2013.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0007850-16.2013.8.21.3001</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>04/03/2013</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Código para download de contracheques no RHE
</commit_message>
<xml_diff>
--- a/Correcao EPROC/Lista de notas.xlsx
+++ b/Correcao EPROC/Lista de notas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,17 +481,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5082691-55.2022.8.21.0001</t>
+          <t>5029547-06.2022.8.21.0022</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5125632-72.2022.8.21.7000/T</t>
+          <t>5007960-93.2020.8.21.0022</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Relacionado no 2o. grau</t>
+          <t>Originário</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>23/05/2022</t>
+          <t>28/09/2022</t>
         </is>
       </c>
     </row>
@@ -526,17 +526,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5001507-82.2021.8.21.0043</t>
+          <t>5002020-12.2020.8.21.0067</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sem dados de processo originário 1</t>
+          <t>9000539-43.2020.8.21.0067</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Nulo</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>27/08/2021</t>
+          <t>03/11/2020</t>
         </is>
       </c>
     </row>
@@ -571,17 +571,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5010754-58.2017.8.21.0001</t>
+          <t>5002025-34.2020.8.21.0067</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0196807-38.2017.8.21.0001</t>
+          <t>9000434-66.2020.8.21.0067</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Digitalizado</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>10/11/2017</t>
+          <t>23/09/2020</t>
         </is>
       </c>
     </row>
@@ -616,17 +616,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5008281-41.2013.8.21.0001</t>
+          <t>5000995-32.2018.8.21.0067</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0087776-25.2013.8.21.0001</t>
+          <t>9000796-39.2018.8.21.0067</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Digitalizado</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>26/12/2011</t>
+          <t>27/11/2018</t>
         </is>
       </c>
     </row>
@@ -661,27 +661,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5001221-76.2018.8.21.0054</t>
+          <t>5002032-26.2020.8.21.0067</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0066578-85.2019.8.21.9000</t>
+          <t>9000450-20.2020.8.21.0067</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Relacionado na TR</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>9000149-83.2018.8.21.0054</t>
+          <t>Sem dados de processo originário 2</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Nulo</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>13/03/2018</t>
+          <t>30/09/2020</t>
         </is>
       </c>
     </row>
@@ -706,17 +706,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5006432-89.2018.8.21.0023</t>
+          <t>5008633-12.2022.8.21.4001</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>9003986-45.2018.8.21.0023</t>
+          <t>5002299-64.2019.8.21.4001</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Originário</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>31/10/2018</t>
+          <t>14/10/2022</t>
         </is>
       </c>
     </row>
@@ -751,17 +751,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5006429-37.2018.8.21.0023</t>
+          <t>5000229-27.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>9003787-23.2018.8.21.0023</t>
+          <t>0420539-74.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>17/10/2018</t>
+          <t>07/12/2011</t>
         </is>
       </c>
     </row>
@@ -796,12 +796,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5009614-96.2011.8.21.0001</t>
+          <t>5000297-74.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0420415-91.2011.8.21.0001</t>
+          <t>0413928-08.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -831,7 +831,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>07/12/2011</t>
+          <t>02/12/2011</t>
         </is>
       </c>
     </row>
@@ -841,12 +841,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5033806-25.2013.8.21.0001</t>
+          <t>5000320-49.2013.8.21.0001</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0007850-16.2013.8.21.3001</t>
+          <t>0044684-94.2013.8.21.0001</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -876,7 +876,412 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>04/03/2013</t>
+          <t>20/02/2013</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>5003815-38.2012.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0023925-46.2012.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>24/01/2012</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>5002031-41.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>9000380-03.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>14/09/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>5002033-11.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>9000365-34.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>09/09/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>5002037-48.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>9000624-29.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>13/11/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>5002090-63.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>9001254-22.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>11/12/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>5002030-56.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>9000405-16.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>18/09/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>5002091-48.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>9001270-73.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>17/12/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>5006127-55.2022.8.21.0059</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>5001247-88.2020.8.21.0059</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Originário</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>19/09/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>5092615-95.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>9015530-62.2019.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>04/04/2019</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adatapação para alterações no site do eproc
</commit_message>
<xml_diff>
--- a/Correcao EPROC/Lista de notas.xlsx
+++ b/Correcao EPROC/Lista de notas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,12 +481,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5029547-06.2022.8.21.0022</t>
+          <t>5008633-12.2022.8.21.4001</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5007960-93.2020.8.21.0022</t>
+          <t>5002299-64.2019.8.21.4001</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>28/09/2022</t>
+          <t>14/10/2022</t>
         </is>
       </c>
     </row>
@@ -526,17 +526,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5002020-12.2020.8.21.0067</t>
+          <t>5006127-55.2022.8.21.0059</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>9000539-43.2020.8.21.0067</t>
+          <t>5001247-88.2020.8.21.0059</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Originário</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>03/11/2020</t>
+          <t>19/09/2022</t>
         </is>
       </c>
     </row>
@@ -571,17 +571,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5002025-34.2020.8.21.0067</t>
+          <t>5157435-21.2022.8.21.0001</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>9000434-66.2020.8.21.0067</t>
+          <t>5032648-85.2020.8.21.0001</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Originário</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>23/09/2020</t>
+          <t>05/09/2022</t>
         </is>
       </c>
     </row>
@@ -616,17 +616,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5000995-32.2018.8.21.0067</t>
+          <t>5026797-60.2023.8.21.0001</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>9000796-39.2018.8.21.0067</t>
+          <t>5030835-67.2013.8.21.0001</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Originário</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>27/11/2018</t>
+          <t>16/02/2023</t>
         </is>
       </c>
     </row>
@@ -661,17 +661,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5002032-26.2020.8.21.0067</t>
+          <t>5035699-12.2017.8.21.0001</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>9000450-20.2020.8.21.0067</t>
+          <t>0161621-51.2017.8.21.0001</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>30/09/2020</t>
+          <t>31/08/2017</t>
         </is>
       </c>
     </row>
@@ -706,17 +706,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5008633-12.2022.8.21.4001</t>
+          <t>5000273-46.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>5002299-64.2019.8.21.4001</t>
+          <t>0420275-57.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Originário</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>14/10/2022</t>
+          <t>07/12/2011</t>
         </is>
       </c>
     </row>
@@ -751,12 +751,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5000229-27.2011.8.21.0001</t>
+          <t>5000274-31.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0420539-74.2011.8.21.0001</t>
+          <t>0413893-48.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>07/12/2011</t>
+          <t>01/12/2011</t>
         </is>
       </c>
     </row>
@@ -796,12 +796,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5000297-74.2011.8.21.0001</t>
+          <t>5004401-12.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0413928-08.2011.8.21.0001</t>
+          <t>0376983-22.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -831,7 +831,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>02/12/2011</t>
+          <t>07/11/2011</t>
         </is>
       </c>
     </row>
@@ -841,12 +841,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5000320-49.2013.8.21.0001</t>
+          <t>5000256-73.2012.8.21.0001</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0044684-94.2013.8.21.0001</t>
+          <t>0023506-26.2012.8.21.0001</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>20/02/2013</t>
+          <t>24/01/2012</t>
         </is>
       </c>
     </row>
@@ -886,12 +886,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5003815-38.2012.8.21.0001</t>
+          <t>5000271-42.2012.8.21.0001</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0023925-46.2012.8.21.0001</t>
+          <t>0351565-48.2012.8.21.0001</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>24/01/2012</t>
+          <t>31/10/2012</t>
         </is>
       </c>
     </row>
@@ -931,17 +931,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5002031-41.2020.8.21.0067</t>
+          <t>5000293-03.2012.8.21.0001</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>9000380-03.2020.8.21.0067</t>
+          <t>0342323-65.2012.8.21.0001</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -966,322 +966,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>14/09/2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>5002033-11.2020.8.21.0067</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>9000365-34.2020.8.21.0067</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>09/09/2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>5002037-48.2020.8.21.0067</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>9000624-29.2020.8.21.0067</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>13/11/2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>5002090-63.2019.8.21.0067</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>9001254-22.2019.8.21.0067</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>11/12/2019</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>5002030-56.2020.8.21.0067</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>9000405-16.2020.8.21.0067</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>18/09/2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>5002091-48.2019.8.21.0067</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>9001270-73.2019.8.21.0067</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>17/12/2019</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>5006127-55.2022.8.21.0059</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>5001247-88.2020.8.21.0059</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Originário</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>19/09/2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>5092615-95.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>9015530-62.2019.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>04/04/2019</t>
+          <t>24/10/2012</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajustes layout correção eproc
</commit_message>
<xml_diff>
--- a/Correcao EPROC/Lista de notas.xlsx
+++ b/Correcao EPROC/Lista de notas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -616,42 +616,42 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5026797-60.2023.8.21.0001</t>
+          <t>5001404-20.2017.8.21.0042</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>5030835-67.2013.8.21.0001</t>
+          <t>0059732-52.2019.8.21.9000</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Originário</t>
+          <t>Relacionado na TR</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Sem dados de processo originário 2</t>
+          <t>9000985-29.2017.8.21.0042</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
           <t>Nulo</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>16/02/2023</t>
+          <t>27/09/2017</t>
         </is>
       </c>
     </row>
@@ -661,312 +661,42 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5035699-12.2017.8.21.0001</t>
+          <t>5001392-06.2017.8.21.0042</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0161621-51.2017.8.21.0001</t>
+          <t>0038543-18.2019.8.21.9000</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Digitalizado</t>
+          <t>Relacionado na TR</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Sem dados de processo originário 2</t>
+          <t>9001086-66.2017.8.21.0042</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>Nulo</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>31/08/2017</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>5000273-46.2011.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>0420275-57.2011.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Digitalizado</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>07/12/2011</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>5000274-31.2011.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0413893-48.2011.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Digitalizado</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>01/12/2011</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>5004401-12.2011.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0376983-22.2011.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Digitalizado</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>07/11/2011</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>5000256-73.2012.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>0023506-26.2012.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Digitalizado</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>24/01/2012</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>5000271-42.2012.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>0351565-48.2012.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Digitalizado</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>31/10/2012</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>5000293-03.2012.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>0342323-65.2012.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Digitalizado</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>24/10/2012</t>
+          <t>05/10/2017</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajustes para sincronizar relatorio e execução. codigo funcionando
</commit_message>
<xml_diff>
--- a/Correcao EPROC/Lista de notas.xlsx
+++ b/Correcao EPROC/Lista de notas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,12 +481,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5008633-12.2022.8.21.4001</t>
+          <t>5216421-65.2022.8.21.0001</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5002299-64.2019.8.21.4001</t>
+          <t>5042179-98.2020.8.21.0001</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>14/10/2022</t>
+          <t>02/12/2022</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5006127-55.2022.8.21.0059</t>
+          <t>5006597-19.2022.8.21.0049</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5001247-88.2020.8.21.0059</t>
+          <t>5002821-79.2020.8.21.0049</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>19/09/2022</t>
+          <t>14/10/2022</t>
         </is>
       </c>
     </row>
@@ -571,17 +571,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5157435-21.2022.8.21.0001</t>
+          <t>5002093-18.2019.8.21.0067</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>5032648-85.2020.8.21.0001</t>
+          <t>9000698-20.2019.8.21.0067</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Originário</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>05/09/2022</t>
+          <t>19/06/2019</t>
         </is>
       </c>
     </row>
@@ -616,27 +616,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5001404-20.2017.8.21.0042</t>
+          <t>5002094-03.2019.8.21.0067</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0059732-52.2019.8.21.9000</t>
+          <t>9001132-09.2019.8.21.0067</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Relacionado na TR</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>9000985-29.2017.8.21.0042</t>
+          <t>Sem dados de processo originário 2</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Nulo</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>27/09/2017</t>
+          <t>21/10/2019</t>
         </is>
       </c>
     </row>
@@ -661,42 +661,852 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5001392-06.2017.8.21.0042</t>
+          <t>5000997-02.2018.8.21.0067</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0038543-18.2019.8.21.9000</t>
+          <t>9000692-47.2018.8.21.0067</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>26/10/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>5002039-18.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>9000407-83.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>18/09/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>5000998-84.2018.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>9000870-93.2018.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>04/12/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>5002095-85.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>9000724-18.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>21/06/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>5002096-70.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>9000532-85.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>04/06/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>5002097-55.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>9000464-38.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>03/06/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>5053427-32.2018.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0046017-06.2020.8.21.9000</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>Relacionado na TR</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>9001086-66.2017.8.21.0042</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>9068801-20.2018.8.21.0001</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
         <is>
           <t>Migrado</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>05/10/2017</t>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>29/11/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>5035085-12.2014.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0395366-43.2014.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>24/11/2014</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>5013439-53.2008.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>1253081-20.2008.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>09/05/2008</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>5013439-53.2008.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1253081-20.2008.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>09/05/2008</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>5013439-53.2008.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1253081-20.2008.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>09/05/2008</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>5013439-53.2008.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>1253081-20.2008.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>09/05/2008</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>5013439-53.2008.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1253081-20.2008.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>09/05/2008</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>5014763-10.2010.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>3103141-73.2010.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>25/11/2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5014763-10.2010.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>3103141-73.2010.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>25/11/2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>5014763-10.2010.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>3103141-73.2010.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>25/11/2010</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>5029278-74.2015.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0199864-35.2015.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>10/08/2015</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>5002539-45.2007.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>3076071-57.2005.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Originário</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0183341-26.2007.8.21.0001</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>31/01/2007</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>5020879-61.2012.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>0026384-42.2012.8.21.3001</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>5063823-92.2023.8.21.0001</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Relacionado</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>5063870-66.2023.8.21.0001</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Relacionado</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>04/09/2012</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Desativação do relatorio email por hack
</commit_message>
<xml_diff>
--- a/Correcao EPROC/Lista de notas.xlsx
+++ b/Correcao EPROC/Lista de notas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,17 +526,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5006597-19.2022.8.21.0049</t>
+          <t>5002825-34.2018.8.21.0002</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5002821-79.2020.8.21.0049</t>
+          <t>9000482-94.2018.8.21.0002</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Originário</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>14/10/2022</t>
+          <t>27/03/2018</t>
         </is>
       </c>
     </row>
@@ -571,17 +571,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5002093-18.2019.8.21.0067</t>
+          <t>5010408-92.2022.8.21.0014</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>9000698-20.2019.8.21.0067</t>
+          <t>5002665-02.2020.8.21.0014</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Originário</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>19/06/2019</t>
+          <t>02/12/2022</t>
         </is>
       </c>
     </row>
@@ -616,17 +616,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5002094-03.2019.8.21.0067</t>
+          <t>5034684-18.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>9001132-09.2019.8.21.0067</t>
+          <t>0111143-49.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>21/10/2019</t>
+          <t>15/04/2011</t>
         </is>
       </c>
     </row>
@@ -661,17 +661,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5000997-02.2018.8.21.0067</t>
+          <t>5029337-62.2015.8.21.0001</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>9000692-47.2018.8.21.0067</t>
+          <t>0090773-10.2015.8.21.0001</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>26/10/2018</t>
+          <t>17/04/2015</t>
         </is>
       </c>
     </row>
@@ -706,17 +706,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5002039-18.2020.8.21.0067</t>
+          <t>5039775-79.2017.8.21.0001</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>9000407-83.2020.8.21.0067</t>
+          <t>0039384-15.2017.8.21.0001</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>18/09/2020</t>
+          <t>14/03/2017</t>
         </is>
       </c>
     </row>
@@ -751,17 +751,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5000998-84.2018.8.21.0067</t>
+          <t>5029499-57.2015.8.21.0001</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>9000870-93.2018.8.21.0067</t>
+          <t>0136341-49.2015.8.21.0001</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>04/12/2018</t>
+          <t>08/06/2015</t>
         </is>
       </c>
     </row>
@@ -796,17 +796,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5002095-85.2019.8.21.0067</t>
+          <t>5028728-21.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>9000724-18.2019.8.21.0067</t>
+          <t>0344069-02.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -831,7 +831,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>21/06/2019</t>
+          <t>19/10/2011</t>
         </is>
       </c>
     </row>
@@ -841,17 +841,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5002096-70.2019.8.21.0067</t>
+          <t>5028728-21.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>9000532-85.2019.8.21.0067</t>
+          <t>0344069-02.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>04/06/2019</t>
+          <t>19/10/2011</t>
         </is>
       </c>
     </row>
@@ -886,12 +886,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5002097-55.2019.8.21.0067</t>
+          <t>5001806-14.2020.8.21.0134</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>9000464-38.2019.8.21.0067</t>
+          <t>9000364-42.2020.8.21.0134</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>03/06/2019</t>
+          <t>06/07/2020</t>
         </is>
       </c>
     </row>
@@ -931,27 +931,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5053427-32.2018.8.21.0001</t>
+          <t>5032111-07.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0046017-06.2020.8.21.9000</t>
+          <t>0111095-90.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Relacionado na TR</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>9068801-20.2018.8.21.0001</t>
+          <t>Sem dados de processo originário 2</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Nulo</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -966,7 +966,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>29/11/2018</t>
+          <t>15/04/2011</t>
         </is>
       </c>
     </row>
@@ -976,12 +976,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5035085-12.2014.8.21.0001</t>
+          <t>5033921-46.2013.8.21.0001</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0395366-43.2014.8.21.0001</t>
+          <t>0037413-34.2013.8.21.0001</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>24/11/2014</t>
+          <t>13/02/2013</t>
         </is>
       </c>
     </row>
@@ -1021,12 +1021,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>5013439-53.2008.8.21.0001</t>
+          <t>5033938-82.2013.8.21.0001</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1253081-20.2008.8.21.0001</t>
+          <t>0084903-52.2013.8.21.0001</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1056,7 +1056,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>09/05/2008</t>
+          <t>28/03/2013</t>
         </is>
       </c>
     </row>
@@ -1066,12 +1066,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>5013439-53.2008.8.21.0001</t>
+          <t>5033938-82.2013.8.21.0001</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1253081-20.2008.8.21.0001</t>
+          <t>0084903-52.2013.8.21.0001</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>09/05/2008</t>
+          <t>28/03/2013</t>
         </is>
       </c>
     </row>
@@ -1111,12 +1111,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5013439-53.2008.8.21.0001</t>
+          <t>5034971-78.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1253081-20.2008.8.21.0001</t>
+          <t>0108702-95.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1146,7 +1146,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>09/05/2008</t>
+          <t>13/04/2011</t>
         </is>
       </c>
     </row>
@@ -1156,12 +1156,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>5013439-53.2008.8.21.0001</t>
+          <t>5034971-78.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1253081-20.2008.8.21.0001</t>
+          <t>0108702-95.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>09/05/2008</t>
+          <t>13/04/2011</t>
         </is>
       </c>
     </row>
@@ -1201,12 +1201,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>5013439-53.2008.8.21.0001</t>
+          <t>5039859-80.2017.8.21.0001</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1253081-20.2008.8.21.0001</t>
+          <t>0129049-42.2017.8.21.0001</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1236,7 +1236,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>09/05/2008</t>
+          <t>06/08/2015</t>
         </is>
       </c>
     </row>
@@ -1246,12 +1246,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>5014763-10.2010.8.21.0001</t>
+          <t>5015478-52.2010.8.21.0001</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>3103141-73.2010.8.21.0001</t>
+          <t>2626731-39.2010.8.21.0001</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>25/11/2010</t>
+          <t>06/10/2010</t>
         </is>
       </c>
     </row>
@@ -1291,12 +1291,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5014763-10.2010.8.21.0001</t>
+          <t>5015600-65.2010.8.21.0001</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>3103141-73.2010.8.21.0001</t>
+          <t>0155171-39.2010.8.21.0001</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1326,7 +1326,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>25/11/2010</t>
+          <t>19/01/2010</t>
         </is>
       </c>
     </row>
@@ -1336,12 +1336,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>5014763-10.2010.8.21.0001</t>
+          <t>5034891-17.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>3103141-73.2010.8.21.0001</t>
+          <t>0243442-87.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>25/11/2010</t>
+          <t>28/07/2011</t>
         </is>
       </c>
     </row>
@@ -1381,12 +1381,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>5029278-74.2015.8.21.0001</t>
+          <t>5034891-17.2011.8.21.0001</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0199864-35.2015.8.21.0001</t>
+          <t>0243442-87.2011.8.21.0001</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>10/08/2015</t>
+          <t>28/07/2011</t>
         </is>
       </c>
     </row>
@@ -1426,27 +1426,27 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>5002539-45.2007.8.21.0001</t>
+          <t>5001001-39.2018.8.21.0067</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>3076071-57.2005.8.21.0001</t>
+          <t>9000812-90.2018.8.21.0067</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Originário</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0183341-26.2007.8.21.0001</t>
+          <t>Sem dados de processo originário 2</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Digitalizado</t>
+          <t>Nulo</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>31/01/2007</t>
+          <t>29/11/2018</t>
         </is>
       </c>
     </row>
@@ -1471,42 +1471,357 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5020879-61.2012.8.21.0001</t>
+          <t>5002047-92.2020.8.21.0067</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0026384-42.2012.8.21.3001</t>
+          <t>9000436-36.2020.8.21.0067</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Digitalizado</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>5063823-92.2023.8.21.0001</t>
+          <t>Sem dados de processo originário 2</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Relacionado</t>
+          <t>Nulo</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>5063870-66.2023.8.21.0001</t>
+          <t>Sem dados de processo originário 3</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Relacionado</t>
+          <t>Nulo</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>04/09/2012</t>
+          <t>24/09/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>5002099-25.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>9000760-60.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>27/06/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>5001002-24.2018.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>9000850-05.2018.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>04/12/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>5002100-10.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>9000786-58.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>03/07/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>5002101-92.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>9000444-47.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>31/05/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>5002102-77.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>9000756-23.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>27/06/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>5002103-62.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>9000754-53.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>27/06/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>5002104-47.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>9000700-87.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>19/06/2019</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adaptacao de credenciais para json
</commit_message>
<xml_diff>
--- a/Correcao EPROC/Lista de notas.xlsx
+++ b/Correcao EPROC/Lista de notas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,12 +481,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5216421-65.2022.8.21.0001</t>
+          <t>5010408-92.2022.8.21.0014</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5042179-98.2020.8.21.0001</t>
+          <t>5002665-02.2020.8.21.0014</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -526,27 +526,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5018241-75.2020.8.21.0033</t>
+          <t>5217136-10.2022.8.21.0001</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0005769-61.2021.8.21.9000</t>
+          <t>5004829-76.2020.8.21.0001</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Relacionado na TR</t>
+          <t>Originário</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>9000749-02.2020.8.21.0033</t>
+          <t>Sem dados de processo originário 2</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Nulo</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>11/02/2020</t>
+          <t>05/12/2022</t>
         </is>
       </c>
     </row>
@@ -571,17 +571,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5010408-92.2022.8.21.0014</t>
+          <t>5006931-56.2021.8.21.0027</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>5002665-02.2020.8.21.0014</t>
+          <t>Sem dados de processo originário 1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Originário</t>
+          <t>Nulo</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>02/12/2022</t>
+          <t>14/04/2021</t>
         </is>
       </c>
     </row>
@@ -616,17 +616,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5006227-49.2006.8.21.0001</t>
+          <t>5000168-66.2021.8.21.0115</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1337741-15.2006.8.21.0001</t>
+          <t>5000168-66.2021.8.21.0115/T</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Digitalizado</t>
+          <t>Relacionado no 2o. grau</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>03/07/2006</t>
+          <t>07/04/2021</t>
         </is>
       </c>
     </row>
@@ -661,27 +661,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5018241-75.2020.8.21.0033</t>
+          <t>5001809-74.2017.8.21.0036</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0005769-61.2021.8.21.9000</t>
+          <t>9002336-55.2017.8.21.0036</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Relacionado na TR</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>9000749-02.2020.8.21.0033</t>
+          <t>Sem dados de processo originário 2</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Nulo</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>11/02/2020</t>
+          <t>23/10/2017</t>
         </is>
       </c>
     </row>
@@ -706,17 +706,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5217136-10.2022.8.21.0001</t>
+          <t>5002735-26.2018.8.21.0002</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>5004829-76.2020.8.21.0001</t>
+          <t>9000271-58.2018.8.21.0002</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Originário</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>05/12/2022</t>
+          <t>09/03/2018</t>
         </is>
       </c>
     </row>
@@ -751,12 +751,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5093406-64.2019.8.21.0001</t>
+          <t>5002731-86.2018.8.21.0002</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>9018514-19.2019.8.21.0001</t>
+          <t>9000433-53.2018.8.21.0002</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>15/04/2019</t>
+          <t>27/03/2018</t>
         </is>
       </c>
     </row>
@@ -796,17 +796,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5005098-47.2023.8.21.0022</t>
+          <t>5035108-55.2014.8.21.0001</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>9003987-96.2019.8.21.0022</t>
+          <t>0028693-44.2014.8.21.0001</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Originário</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -831,7 +831,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>28/02/2023</t>
+          <t>28/01/2014</t>
         </is>
       </c>
     </row>
@@ -841,17 +841,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5093438-69.2019.8.21.0001</t>
+          <t>5035108-55.2014.8.21.0001</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>9020456-86.2019.8.21.0001</t>
+          <t>0028693-44.2014.8.21.0001</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>22/04/2019</t>
+          <t>28/01/2014</t>
         </is>
       </c>
     </row>
@@ -886,42 +886,1032 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5093440-39.2019.8.21.0001</t>
+          <t>5035108-55.2014.8.21.0001</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>9021532-48.2019.8.21.0001</t>
+          <t>0028693-44.2014.8.21.0001</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>28/01/2014</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>5035108-55.2014.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0028693-44.2014.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>28/01/2014</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>5009658-08.2018.8.21.0022</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>9003683-34.2018.8.21.0022</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>Migrado</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>24/04/2019</t>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>30/05/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>5002111-39.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>9000482-59.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>03/06/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>5002115-76.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>9001255-07.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>11/12/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>5001005-76.2018.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>9000856-12.2018.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>04/12/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>5002061-76.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>9000182-63.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>06/04/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>5002116-61.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>9000433-18.2019.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>31/05/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>5002062-61.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>9000400-91.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>17/09/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>5001006-61.2018.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>9000817-15.2018.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>29/11/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>5002063-46.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>9000178-26.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>06/04/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>5002065-16.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>9000388-77.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>16/09/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>5001007-46.2018.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>9000790-32.2018.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>27/11/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>5002068-68.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>9000458-94.2020.8.21.0067</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>05/10/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>5000282-08.2011.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>0302109-66.2011.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>18/08/2011</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>5034992-20.2012.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0303805-06.2012.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>13/09/2012</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>5008342-82.2022.8.21.0033</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>9001156-08.2020.8.21.0033</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Originário</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>22/04/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>5009659-90.2018.8.21.0022</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>9005551-47.2018.8.21.0022</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>31/07/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>5029547-06.2022.8.21.0022</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>5007960-93.2020.8.21.0022</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Originário</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>28/09/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>5002741-33.2018.8.21.0002</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>9000456-96.2018.8.21.0002</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>27/03/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>5008759-20.2011.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0148964-87.2011.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>16/05/2011</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>5019558-25.2011.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>0218063-47.2011.8.21.0001</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Digitalizado</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>22/06/2011</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>5125809-52.2020.8.21.0001</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>9001529-57.2020.8.21.0027</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Migrado</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 2</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Sem dados de processo originário 3</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Nulo</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>18/05/2020</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Correção do envio de emails e esboço para quebrar captcha
</commit_message>
<xml_diff>
--- a/Correcao EPROC/Lista de notas.xlsx
+++ b/Correcao EPROC/Lista de notas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -661,17 +661,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5001809-74.2017.8.21.0036</t>
+          <t>5015948-83.2010.8.21.0001</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>9002336-55.2017.8.21.0036</t>
+          <t>1999701-78.2010.8.21.0001</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>23/10/2017</t>
+          <t>03/08/2010</t>
         </is>
       </c>
     </row>
@@ -706,17 +706,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5002735-26.2018.8.21.0002</t>
+          <t>5015948-83.2010.8.21.0001</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>9000271-58.2018.8.21.0002</t>
+          <t>1999701-78.2010.8.21.0001</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>09/03/2018</t>
+          <t>03/08/2010</t>
         </is>
       </c>
     </row>
@@ -751,17 +751,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5002731-86.2018.8.21.0002</t>
+          <t>5015948-83.2010.8.21.0001</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>9000433-53.2018.8.21.0002</t>
+          <t>1999701-78.2010.8.21.0001</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>27/03/2018</t>
+          <t>03/08/2010</t>
         </is>
       </c>
     </row>
@@ -796,17 +796,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5035108-55.2014.8.21.0001</t>
+          <t>5008342-82.2022.8.21.0033</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0028693-44.2014.8.21.0001</t>
+          <t>9001156-08.2020.8.21.0033</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Digitalizado</t>
+          <t>Originário</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -831,7 +831,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>28/01/2014</t>
+          <t>22/04/2022</t>
         </is>
       </c>
     </row>
@@ -841,17 +841,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5035108-55.2014.8.21.0001</t>
+          <t>5029547-06.2022.8.21.0022</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0028693-44.2014.8.21.0001</t>
+          <t>5007960-93.2020.8.21.0022</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Digitalizado</t>
+          <t>Originário</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>28/01/2014</t>
+          <t>28/09/2022</t>
         </is>
       </c>
     </row>
@@ -886,17 +886,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5035108-55.2014.8.21.0001</t>
+          <t>5002368-19.2021.8.21.0027</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0028693-44.2014.8.21.0001</t>
+          <t>Sem dados de processo originário 1</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Digitalizado</t>
+          <t>Nulo</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>28/01/2014</t>
+          <t>09/02/2021</t>
         </is>
       </c>
     </row>
@@ -931,17 +931,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5035108-55.2014.8.21.0001</t>
+          <t>5016829-79.2019.8.21.0022</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0028693-44.2014.8.21.0001</t>
+          <t>9000968-82.2019.8.21.0022</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Digitalizado</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -966,7 +966,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>28/01/2014</t>
+          <t>19/02/2019</t>
         </is>
       </c>
     </row>
@@ -976,29 +976,29 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5009658-08.2018.8.21.0022</t>
+          <t>5016824-57.2019.8.21.0022</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>9003683-34.2018.8.21.0022</t>
+          <t>0010252-71.2020.8.21.9000/T</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t>Relacionado no 2o. grau</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>9007972-73.2019.8.21.0022</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
           <t>Migrado</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
       <c r="G13" t="inlineStr">
         <is>
           <t>Sem dados de processo originário 3</t>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>30/05/2018</t>
+          <t>01/11/2019</t>
         </is>
       </c>
     </row>
@@ -1021,29 +1021,29 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>5002111-39.2019.8.21.0067</t>
+          <t>5009671-07.2018.8.21.0022</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>9000482-59.2019.8.21.0067</t>
+          <t>0006807-45.2020.8.21.9000/T</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>Relacionado no 2o. grau</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>9009420-18.2018.8.21.0022</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>Migrado</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
       <c r="G14" t="inlineStr">
         <is>
           <t>Sem dados de processo originário 3</t>
@@ -1056,7 +1056,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>03/06/2019</t>
+          <t>03/12/2018</t>
         </is>
       </c>
     </row>
@@ -1066,12 +1066,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>5002115-76.2019.8.21.0067</t>
+          <t>5009668-52.2018.8.21.0022</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>9001255-07.2019.8.21.0067</t>
+          <t>9009424-55.2018.8.21.0022</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>11/12/2019</t>
+          <t>03/12/2018</t>
         </is>
       </c>
     </row>
@@ -1111,29 +1111,29 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5001005-76.2018.8.21.0067</t>
+          <t>5009667-67.2018.8.21.0022</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>9000856-12.2018.8.21.0067</t>
+          <t>0014717-60.2019.8.21.9000/T</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>Relacionado no 2o. grau</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>9008752-47.2018.8.21.0022</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
           <t>Migrado</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
       <c r="G16" t="inlineStr">
         <is>
           <t>Sem dados de processo originário 3</t>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>04/12/2018</t>
+          <t>08/11/2018</t>
         </is>
       </c>
     </row>
@@ -1156,29 +1156,29 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>5002061-76.2020.8.21.0067</t>
+          <t>5009665-97.2018.8.21.0022</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>9000182-63.2020.8.21.0067</t>
+          <t>0015900-66.2019.8.21.9000/T</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>Relacionado no 2o. grau</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>9009358-75.2018.8.21.0022</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>Migrado</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
       <c r="G17" t="inlineStr">
         <is>
           <t>Sem dados de processo originário 3</t>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>06/04/2020</t>
+          <t>30/11/2018</t>
         </is>
       </c>
     </row>
@@ -1201,29 +1201,29 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>5002116-61.2019.8.21.0067</t>
+          <t>5009663-30.2018.8.21.0022</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>9000433-18.2019.8.21.0067</t>
+          <t>0009759-31.2019.8.21.9000/T</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>Relacionado no 2o. grau</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>9007912-37.2018.8.21.0022</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>Migrado</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
       <c r="G18" t="inlineStr">
         <is>
           <t>Sem dados de processo originário 3</t>
@@ -1236,7 +1236,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>31/05/2019</t>
+          <t>11/10/2018</t>
         </is>
       </c>
     </row>
@@ -1246,12 +1246,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>5002062-61.2020.8.21.0067</t>
+          <t>5001397-28.2017.8.21.0042</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>9000400-91.2020.8.21.0067</t>
+          <t>9001059-83.2017.8.21.0042</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>17/09/2020</t>
+          <t>29/09/2017</t>
         </is>
       </c>
     </row>
@@ -1291,17 +1291,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>5001006-61.2018.8.21.0067</t>
+          <t>5072049-91.2020.8.21.0001</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>9000817-15.2018.8.21.0067</t>
+          <t>3221931-89.2005.8.21.0001</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Migrado</t>
+          <t>Digitalizado</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1326,592 +1326,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>29/11/2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>5002063-46.2020.8.21.0067</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>9000178-26.2020.8.21.0067</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>06/04/2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>5002065-16.2020.8.21.0067</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>9000388-77.2020.8.21.0067</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>16/09/2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>5001007-46.2018.8.21.0067</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>9000790-32.2018.8.21.0067</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>27/11/2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>5002068-68.2020.8.21.0067</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>9000458-94.2020.8.21.0067</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>05/10/2020</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>5000282-08.2011.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>0302109-66.2011.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Digitalizado</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>18/08/2011</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>5034992-20.2012.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>0303805-06.2012.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Digitalizado</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>13/09/2012</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>5008342-82.2022.8.21.0033</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>9001156-08.2020.8.21.0033</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Originário</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>22/04/2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>5009659-90.2018.8.21.0022</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>9005551-47.2018.8.21.0022</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>31/07/2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>5029547-06.2022.8.21.0022</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>5007960-93.2020.8.21.0022</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Originário</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>28/09/2022</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>5002741-33.2018.8.21.0002</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>9000456-96.2018.8.21.0002</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>27/03/2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>5008759-20.2011.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>0148964-87.2011.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Digitalizado</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>16/05/2011</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>5019558-25.2011.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>0218063-47.2011.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Digitalizado</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>22/06/2011</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>5125809-52.2020.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>9001529-57.2020.8.21.0027</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>18/05/2020</t>
+          <t>22/10/2004</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Criando codigo para quebrar captcha
</commit_message>
<xml_diff>
--- a/Correcao EPROC/Lista de notas.xlsx
+++ b/Correcao EPROC/Lista de notas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,12 +481,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>5010408-92.2022.8.21.0014</t>
+          <t>5202537-66.2022.8.21.0001</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5002665-02.2020.8.21.0014</t>
+          <t>5012652-04.2020.8.21.0001</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>02/12/2022</t>
+          <t>11/11/2022</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>5217136-10.2022.8.21.0001</t>
+          <t>5168190-07.2022.8.21.0001</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5004829-76.2020.8.21.0001</t>
+          <t>5016585-82.2020.8.21.0001</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>05/12/2022</t>
+          <t>22/09/2022</t>
         </is>
       </c>
     </row>
@@ -571,17 +571,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5006931-56.2021.8.21.0027</t>
+          <t>5001327-37.2021.8.21.0085</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Sem dados de processo originário 1</t>
+          <t>9000091-79.2021.8.21.0085</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Nulo</t>
+          <t>Migrado</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>14/04/2021</t>
+          <t>13/05/2021</t>
         </is>
       </c>
     </row>
@@ -616,17 +616,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5000168-66.2021.8.21.0115</t>
+          <t>5031950-45.2021.8.21.0001</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>5000168-66.2021.8.21.0115/T</t>
+          <t>Sem dados de processo originário 1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Relacionado no 2o. grau</t>
+          <t>Nulo</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>07/04/2021</t>
+          <t>30/03/2021</t>
         </is>
       </c>
     </row>
@@ -661,17 +661,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5015948-83.2010.8.21.0001</t>
+          <t>5082691-55.2022.8.21.0001</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1999701-78.2010.8.21.0001</t>
+          <t>5125632-72.2022.8.21.7000/T</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Digitalizado</t>
+          <t>Relacionado no 2o. grau</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>03/08/2010</t>
+          <t>23/05/2022</t>
         </is>
       </c>
     </row>
@@ -706,12 +706,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5015948-83.2010.8.21.0001</t>
+          <t>5003574-61.2017.8.21.0010</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1999701-78.2010.8.21.0001</t>
+          <t>0020708-89.2017.8.21.0010</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -721,12 +721,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Sem dados de processo originário 2</t>
+          <t>5024835-77.2020.8.21.0010</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Nulo</t>
+          <t>Apenso</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>03/08/2010</t>
+          <t>11/05/2017</t>
         </is>
       </c>
     </row>
@@ -751,17 +751,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5015948-83.2010.8.21.0001</t>
+          <t>5008633-12.2022.8.21.4001</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1999701-78.2010.8.21.0001</t>
+          <t>5002299-64.2019.8.21.4001</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Digitalizado</t>
+          <t>Originário</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>03/08/2010</t>
+          <t>14/10/2022</t>
         </is>
       </c>
     </row>
@@ -796,12 +796,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5008342-82.2022.8.21.0033</t>
+          <t>5008633-12.2022.8.21.4001</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>9001156-08.2020.8.21.0033</t>
+          <t>5002299-64.2019.8.21.4001</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -831,7 +831,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>22/04/2022</t>
+          <t>14/10/2022</t>
         </is>
       </c>
     </row>
@@ -841,12 +841,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>5029547-06.2022.8.21.0022</t>
+          <t>5011085-85.2022.8.21.3001</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>5007960-93.2020.8.21.0022</t>
+          <t>5000119-97.2021.8.21.3001</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -856,12 +856,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Sem dados de processo originário 2</t>
+          <t>5025664-35.2023.8.21.7000/T</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Nulo</t>
+          <t>Relacionado no 2o. grau</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>28/09/2022</t>
+          <t>05/10/2022</t>
         </is>
       </c>
     </row>
@@ -886,17 +886,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5002368-19.2021.8.21.0027</t>
+          <t>5010628-20.2022.8.21.0005</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Sem dados de processo originário 1</t>
+          <t>5003354-73.2020.8.21.0005</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Nulo</t>
+          <t>Originário</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -921,412 +921,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>09/02/2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>5016829-79.2019.8.21.0022</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>9000968-82.2019.8.21.0022</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>19/02/2019</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>5016824-57.2019.8.21.0022</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>0010252-71.2020.8.21.9000/T</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Relacionado no 2o. grau</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>9007972-73.2019.8.21.0022</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>01/11/2019</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>5009671-07.2018.8.21.0022</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>0006807-45.2020.8.21.9000/T</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Relacionado no 2o. grau</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>9009420-18.2018.8.21.0022</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>03/12/2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>5009668-52.2018.8.21.0022</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>9009424-55.2018.8.21.0022</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>03/12/2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>5009667-67.2018.8.21.0022</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>0014717-60.2019.8.21.9000/T</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Relacionado no 2o. grau</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>9008752-47.2018.8.21.0022</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>08/11/2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>5009665-97.2018.8.21.0022</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>0015900-66.2019.8.21.9000/T</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Relacionado no 2o. grau</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>9009358-75.2018.8.21.0022</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>30/11/2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>5009663-30.2018.8.21.0022</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>0009759-31.2019.8.21.9000/T</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Relacionado no 2o. grau</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>9007912-37.2018.8.21.0022</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>11/10/2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>5001397-28.2017.8.21.0042</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>9001059-83.2017.8.21.0042</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Migrado</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>29/09/2017</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>5072049-91.2020.8.21.0001</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>3221931-89.2005.8.21.0001</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Digitalizado</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 2</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Sem dados de processo originário 3</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Nulo</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>22/10/2004</t>
+          <t>13/09/2022</t>
         </is>
       </c>
     </row>

</xml_diff>